<commit_message>
finished chapter 17. Added new (crappy) project.. maybe i will delete it in future..
</commit_message>
<xml_diff>
--- a/Maschinelles Lernen/Glossar Notizen.xlsx
+++ b/Maschinelles Lernen/Glossar Notizen.xlsx
@@ -1,56 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Allgemeine_Dokumente\Maschinelles Lernen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6128C82A-95E7-476D-9B07-3695CDBD6EC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="8985" yWindow="6720" windowWidth="37995" windowHeight="15885" xr2:uid="{DF36CCE8-B822-40A4-BD4C-9CE353A9C120}"/>
+    <workbookView windowHeight="18450"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+  <si>
+    <t>Nr.</t>
+  </si>
   <si>
     <t>Wörter für das Glossar</t>
   </si>
   <si>
+    <t>Kapitel</t>
+  </si>
+  <si>
+    <t>Anmerkung</t>
+  </si>
+  <si>
     <t>Cluster</t>
   </si>
   <si>
-    <t>Kapitel</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 15.2</t>
   </si>
   <si>
-    <t>Nr.</t>
-  </si>
-  <si>
     <t>Input</t>
   </si>
   <si>
+    <t>https://missinglink.ai/guides/neural-network-concepts/complete-guide-artificial-neural-networks/</t>
+  </si>
+  <si>
     <t>Trainingssatz</t>
   </si>
   <si>
@@ -66,12 +55,6 @@
     <t>Forward Pass</t>
   </si>
   <si>
-    <t>Anmerkung</t>
-  </si>
-  <si>
-    <t>https://missinglink.ai/guides/neural-network-concepts/complete-guide-artificial-neural-networks/</t>
-  </si>
-  <si>
     <t>Error/loss/Fehler</t>
   </si>
   <si>
@@ -103,18 +86,33 @@
   </si>
   <si>
     <t>semi-überwachtes Lernen</t>
+  </si>
+  <si>
+    <t>pseudo-labeling</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>Data Augmentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,19 +120,349 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -142,29 +470,315 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Komma" xfId="2" builtinId="3"/>
+    <cellStyle name="40% - Akzent4" xfId="3" builtinId="43"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9"/>
+    <cellStyle name="Akzent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Währung" xfId="6" builtinId="4"/>
+    <cellStyle name="Prozent" xfId="7" builtinId="5"/>
+    <cellStyle name="Akzent4" xfId="8" builtinId="41"/>
+    <cellStyle name="Komma[0]" xfId="9" builtinId="6"/>
+    <cellStyle name="Eingabe" xfId="10" builtinId="20"/>
+    <cellStyle name="Hinweis" xfId="11" builtinId="10"/>
+    <cellStyle name="Währung[0]" xfId="12" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8"/>
+    <cellStyle name="Warnmeldung" xfId="14" builtinId="11"/>
+    <cellStyle name="Akzent5" xfId="15" builtinId="45"/>
+    <cellStyle name="Titel" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Überschrift 2" xfId="18" builtinId="17"/>
+    <cellStyle name="Überschrift 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Überschrift 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Ausgabe" xfId="21" builtinId="21"/>
+    <cellStyle name="40% - Akzent2" xfId="22" builtinId="35"/>
+    <cellStyle name="Gesamt" xfId="23" builtinId="25"/>
+    <cellStyle name="Berechnung" xfId="24" builtinId="22"/>
+    <cellStyle name="Zelle überprüfen" xfId="25" builtinId="23"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="26" builtinId="24"/>
+    <cellStyle name="Gut" xfId="27" builtinId="26"/>
+    <cellStyle name="40% - Akzent3" xfId="28" builtinId="39"/>
+    <cellStyle name="Schlecht" xfId="29" builtinId="27"/>
+    <cellStyle name="60% - Akzent6" xfId="30" builtinId="52"/>
+    <cellStyle name="Neutral" xfId="31" builtinId="28"/>
+    <cellStyle name="Akzent1" xfId="32" builtinId="29"/>
+    <cellStyle name="20% - Akzent1" xfId="33" builtinId="30"/>
+    <cellStyle name="40% - Akzent1" xfId="34" builtinId="31"/>
+    <cellStyle name="20% - Akzent5" xfId="35" builtinId="46"/>
+    <cellStyle name="60% - Akzent1" xfId="36" builtinId="32"/>
+    <cellStyle name="20% - Akzent2" xfId="37" builtinId="34"/>
+    <cellStyle name="20% - Akzent6" xfId="38" builtinId="50"/>
+    <cellStyle name="60% - Akzent2" xfId="39" builtinId="36"/>
+    <cellStyle name="Akzent3" xfId="40" builtinId="37"/>
+    <cellStyle name="20% - Akzent3" xfId="41" builtinId="38"/>
+    <cellStyle name="60% - Akzent3" xfId="42" builtinId="40"/>
+    <cellStyle name="20% - Akzent4" xfId="43" builtinId="42"/>
+    <cellStyle name="60% - Akzent4" xfId="44" builtinId="44"/>
+    <cellStyle name="40% - Akzent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Akzent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Akzent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Akzent6" xfId="48" builtinId="51"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -213,7 +827,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -246,26 +860,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -298,23 +895,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -456,228 +1036,236 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3258C06-0AE5-42D0-A0B9-D91871C092CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="24.2857142857143" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="C14" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
finished chapter 22 (?) (or 21... ka mehr)
</commit_message>
<xml_diff>
--- a/Maschinelles Lernen/Glossar Notizen.xlsx
+++ b/Maschinelles Lernen/Glossar Notizen.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Allgemeine_Dokumente\Maschinelles Lernen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC08973-C99A-42D6-94E2-DF40FB440696}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="-120" windowWidth="50700" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="21000" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Nr.</t>
   </si>
@@ -122,13 +116,28 @@
   </si>
   <si>
     <t>Zero Padding</t>
+  </si>
+  <si>
+    <t>Bias</t>
+  </si>
+  <si>
+    <t>Gradient/Ableitung</t>
+  </si>
+  <si>
+    <t>Ableitung: https://www.mathelounge.de/1981/was-ist-eine-ableitung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,16 +153,346 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -161,9 +500,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -171,19 +752,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Komma" xfId="2" builtinId="3"/>
+    <cellStyle name="40% - Akzent4" xfId="3" builtinId="43"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9"/>
+    <cellStyle name="Akzent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Währung" xfId="6" builtinId="4"/>
+    <cellStyle name="Prozent" xfId="7" builtinId="5"/>
+    <cellStyle name="Akzent4" xfId="8" builtinId="41"/>
+    <cellStyle name="Komma[0]" xfId="9" builtinId="6"/>
+    <cellStyle name="Eingabe" xfId="10" builtinId="20"/>
+    <cellStyle name="Hinweis" xfId="11" builtinId="10"/>
+    <cellStyle name="Währung[0]" xfId="12" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8"/>
+    <cellStyle name="Warnmeldung" xfId="14" builtinId="11"/>
+    <cellStyle name="Akzent5" xfId="15" builtinId="45"/>
+    <cellStyle name="Titel" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Überschrift 2" xfId="18" builtinId="17"/>
+    <cellStyle name="Überschrift 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Überschrift 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Ausgabe" xfId="21" builtinId="21"/>
+    <cellStyle name="40% - Akzent2" xfId="22" builtinId="35"/>
+    <cellStyle name="Gesamt" xfId="23" builtinId="25"/>
+    <cellStyle name="Berechnung" xfId="24" builtinId="22"/>
+    <cellStyle name="Zelle überprüfen" xfId="25" builtinId="23"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="26" builtinId="24"/>
+    <cellStyle name="Gut" xfId="27" builtinId="26"/>
+    <cellStyle name="40% - Akzent3" xfId="28" builtinId="39"/>
+    <cellStyle name="Schlecht" xfId="29" builtinId="27"/>
+    <cellStyle name="60% - Akzent6" xfId="30" builtinId="52"/>
+    <cellStyle name="Neutral" xfId="31" builtinId="28"/>
+    <cellStyle name="Akzent1" xfId="32" builtinId="29"/>
+    <cellStyle name="20% - Akzent1" xfId="33" builtinId="30"/>
+    <cellStyle name="40% - Akzent1" xfId="34" builtinId="31"/>
+    <cellStyle name="20% - Akzent5" xfId="35" builtinId="46"/>
+    <cellStyle name="60% - Akzent1" xfId="36" builtinId="32"/>
+    <cellStyle name="20% - Akzent2" xfId="37" builtinId="34"/>
+    <cellStyle name="20% - Akzent6" xfId="38" builtinId="50"/>
+    <cellStyle name="60% - Akzent2" xfId="39" builtinId="36"/>
+    <cellStyle name="Akzent3" xfId="40" builtinId="37"/>
+    <cellStyle name="20% - Akzent3" xfId="41" builtinId="38"/>
+    <cellStyle name="60% - Akzent3" xfId="42" builtinId="40"/>
+    <cellStyle name="20% - Akzent4" xfId="43" builtinId="42"/>
+    <cellStyle name="60% - Akzent4" xfId="44" builtinId="44"/>
+    <cellStyle name="40% - Akzent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Akzent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Akzent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Akzent6" xfId="48" builtinId="51"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -441,22 +1066,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="24.2857142857143" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -473,7 +1098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -600,7 +1225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -608,7 +1233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -619,7 +1244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -627,7 +1252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -635,7 +1260,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -643,7 +1268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -654,7 +1279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -665,7 +1290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -676,7 +1301,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -704,7 +1329,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -715,9 +1340,29 @@
         <v>20</v>
       </c>
     </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <ignoredErrors>
     <ignoredError sqref="C14" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
started chapter 25 (i guess.. or 24..)
</commit_message>
<xml_diff>
--- a/Maschinelles Lernen/Glossar Notizen.xlsx
+++ b/Maschinelles Lernen/Glossar Notizen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Allgemeine_Dokumente\Maschinelles Lernen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA6D64C-2F0F-4A1B-AF95-71BD8C5A09ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4433391-0437-42FD-9FB7-4B461E2B4E8B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6495" yWindow="7770" windowWidth="37785" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4284" yWindow="3072" windowWidth="16368" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Nr.</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>fully connected</t>
+  </si>
+  <si>
+    <t>Siehe concolutional Layer</t>
+  </si>
+  <si>
+    <t>Kernel/Filter</t>
   </si>
 </sst>
 </file>
@@ -484,16 +490,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1"/>
   </cols>
   <sheetData>
@@ -816,6 +822,17 @@
         <v>43</v>
       </c>
     </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished chapter 29, startet chapter 30
</commit_message>
<xml_diff>
--- a/Maschinelles Lernen/Glossar Notizen.xlsx
+++ b/Maschinelles Lernen/Glossar Notizen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Allgemeine_Dokumente\Maschinelles Lernen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FCC23D-A9F9-435E-BF06-6C73A046CC64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFE9188-1938-4708-9C34-F8BDD41DD264}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7605" yWindow="11130" windowWidth="37785" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="768" windowWidth="16368" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Nr.</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Beim übergeben von einem conv layer an einen Dense muss geflatted werden</t>
+  </si>
+  <si>
+    <t>Varianz</t>
+  </si>
+  <si>
+    <t>zb 28, aber vorher a scho sicher</t>
   </si>
 </sst>
 </file>
@@ -506,16 +512,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="1"/>
   </cols>
   <sheetData>
@@ -874,6 +880,17 @@
         <v>50</v>
       </c>
     </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished chapter 31 -> finished all chapters :)
</commit_message>
<xml_diff>
--- a/Maschinelles Lernen/Glossar Notizen.xlsx
+++ b/Maschinelles Lernen/Glossar Notizen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Allgemeine_Dokumente\Maschinelles Lernen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E138E66F-7119-4335-8E8F-502AACA31B0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4517D371-3A96-4A72-B168-34D44866C785}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3372" yWindow="1512" windowWidth="16368" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">30.2.1 </t>
   </si>
   <si>
-    <t>Batch norm</t>
+    <t>Batch norm/Batch Normalization</t>
   </si>
 </sst>
 </file>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.4"/>

</xml_diff>